<commit_message>
added date, location, diurnal to earthquakes db. fixed timezone. added locatoincomponents table and joinable data to earthquakes data. now using day feed from usgs.
</commit_message>
<xml_diff>
--- a/Stats.xlsx
+++ b/Stats.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david/Dropbox/Development/PHP/Earthquakes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{58870924-D15F-9E44-8F1E-C88147205439}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6EFD7F-2019-A746-8300-3B68A4A190DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14780" yWindow="4140" windowWidth="23620" windowHeight="15320" xr2:uid="{FCEDE3B9-7684-D241-B186-58B2BB124BAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
   <si>
     <t>2000+ 9</t>
   </si>
@@ -171,12 +171,6 @@
   </si>
   <si>
     <t>volcanic eruption</t>
-  </si>
-  <si>
-    <t>=SUM(H1:H25)</t>
-  </si>
-  <si>
-    <t>=sum(H1:H25</t>
   </si>
 </sst>
 </file>
@@ -218,11 +212,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB5C3C38-4D49-FB4C-B42E-29091401F72F}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -549,7 +545,7 @@
     <col min="2" max="2" width="10.83203125" style="2"/>
     <col min="4" max="4" width="10.83203125" style="2"/>
     <col min="7" max="7" width="26.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="1"/>
+    <col min="8" max="9" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -562,7 +558,7 @@
       <c r="G1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="3">
+      <c r="H1" s="4">
         <v>2</v>
       </c>
     </row>
@@ -576,7 +572,7 @@
       <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="4">
         <v>5</v>
       </c>
     </row>
@@ -590,7 +586,7 @@
       <c r="G3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="4">
         <v>407</v>
       </c>
     </row>
@@ -604,7 +600,7 @@
       <c r="G4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="4">
         <v>1</v>
       </c>
     </row>
@@ -618,7 +614,7 @@
       <c r="G5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="4">
         <v>3748166</v>
       </c>
     </row>
@@ -632,7 +628,7 @@
       <c r="G6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="4">
         <v>5</v>
       </c>
     </row>
@@ -646,7 +642,7 @@
       <c r="G7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="4">
         <v>23425</v>
       </c>
     </row>
@@ -660,7 +656,7 @@
       <c r="G8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="4">
         <v>11149</v>
       </c>
     </row>
@@ -677,7 +673,7 @@
       <c r="G9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="4">
         <v>1</v>
       </c>
     </row>
@@ -702,7 +698,7 @@
       <c r="G10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="4">
         <v>1</v>
       </c>
     </row>
@@ -716,7 +712,7 @@
       <c r="G11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="4">
         <v>16</v>
       </c>
     </row>
@@ -730,7 +726,7 @@
       <c r="G12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="4">
         <v>1</v>
       </c>
     </row>
@@ -744,7 +740,7 @@
       <c r="G13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="4">
         <v>37</v>
       </c>
     </row>
@@ -758,7 +754,7 @@
       <c r="G14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H14" s="4">
         <v>1554</v>
       </c>
     </row>
@@ -772,7 +768,7 @@
       <c r="G15" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H15" s="4">
         <v>3</v>
       </c>
     </row>
@@ -786,11 +782,11 @@
       <c r="G16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H16" s="4">
         <v>1086</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>6</v>
       </c>
@@ -800,11 +796,11 @@
       <c r="G17" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="4">
         <v>1471</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
@@ -814,11 +810,11 @@
       <c r="G18" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="4">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -831,11 +827,11 @@
       <c r="G19" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H19" s="4">
         <v>64033</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>0</v>
       </c>
@@ -856,11 +852,11 @@
       <c r="G20" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H20" s="4">
         <v>183</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <f>SUM(B1:B20)</f>
         <v>3505188</v>
@@ -876,48 +872,54 @@
       <c r="G21" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H21" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="G22" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="4">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="G23" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H23" s="4">
         <v>361</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="G24" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H24" s="4">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="G25" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H25" s="3">
+      <c r="H25" s="4">
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="H26" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>46</v>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="H26" s="2">
+        <f>SUM(H1:H25)</f>
+        <v>103827</v>
+      </c>
+      <c r="I26" s="2">
+        <f>SUM(I1:I25)</f>
+        <v>3748166</v>
+      </c>
+      <c r="J26" s="5">
+        <f>H26/I26</f>
+        <v>2.770074751224999E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>